<commit_message>
Made some changes to my file
</commit_message>
<xml_diff>
--- a/Movies DB_Solutions.xlsx
+++ b/Movies DB_Solutions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\codar\excel files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\codar\excel files\Movies DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D4B1B7-1263-4DBF-8CCC-39150309C083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2B5338-3DD3-4DD5-9B6B-2DB178ECFA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="4" xr2:uid="{24D39405-1A2E-4110-AFA3-BEC10B9E0557}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{24D39405-1A2E-4110-AFA3-BEC10B9E0557}"/>
   </bookViews>
   <sheets>
     <sheet name="Charts and Tables" sheetId="6" r:id="rId1"/>
@@ -28,8 +28,8 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId8"/>
-    <pivotCache cacheId="6" r:id="rId9"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="79">
   <si>
     <t>MOVIE</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>3. Movie Summary</t>
+  </si>
+  <si>
+    <t>This is a change</t>
   </si>
 </sst>
 </file>
@@ -628,11 +631,19 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -642,9 +653,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -784,11 +792,6 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -814,10 +817,10 @@
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.0"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
@@ -5166,6 +5169,15 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
+          <c:showLegendKey val="1"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="1"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
@@ -5207,6 +5219,15 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
+          <c:showLegendKey val="1"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="1"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
@@ -5248,6 +5269,15 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
+          <c:showLegendKey val="1"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="1"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
@@ -5701,6 +5731,36 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-0457-40F1-8A99-6AD5AA550283}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-0457-40F1-8A99-6AD5AA550283}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-0457-40F1-8A99-6AD5AA550283}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="2"/>
@@ -11912,8 +11972,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>79376</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="10" name="Average Status">
@@ -11936,7 +11996,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -12881,7 +12941,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6A02599F-D8EA-476C-8786-E3483257E9B7}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6A02599F-D8EA-476C-8786-E3483257E9B7}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B3:D11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -12980,7 +13040,1197 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2D4E6CDA-203E-4D14-B3EC-C27B3E2A842C}" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4D9962DE-38CB-4034-A1F8-9ADCEFCAE6F3}" name="PivotTable9" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="J26" firstHeaderRow="0" firstDataRow="0" firstDataCol="0" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="16">
+    <pivotField axis="axisPage" showAll="0">
+      <items count="17">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="9"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="10"/>
+        <item x="8"/>
+        <item x="14"/>
+        <item x="12"/>
+        <item x="3"/>
+        <item x="15"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="9" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <pageFields count="1">
+    <pageField fld="0" hier="-1"/>
+  </pageFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0D4AFFF-2BFF-415B-98D2-4EC608BED0AA}" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+  <location ref="J16:J17" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField compact="0" showAll="0"/>
+    <pivotField compact="0" showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="164" showAll="0">
+      <items count="15">
+        <item x="13"/>
+        <item x="12"/>
+        <item x="11"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="9" showAll="0"/>
+    <pivotField compact="0" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="10" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="7">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6B138F6B-7AFC-4CD2-A1A3-926BBE22CE78}" name="PivotTable4" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="J2:K9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0">
+      <items count="15">
+        <item x="13"/>
+        <item x="12"/>
+        <item x="11"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="9" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+    <i i="6">
+      <x v="6"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="7">
+    <dataField name="Average of Jul-21" fld="3" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of Aug-21" fld="4" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of Sep-21" fld="5" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of Oct-21" fld="6" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of Nov-21" fld="7" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of Dec-21" fld="8" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of Jan-22" fld="9" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="8">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="2" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F156695-00A6-4622-942C-8A4E46F4AA06}" name="PivotTable6" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="J21:J22" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="9" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Average" fld="11" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="9">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D4BBF573-D747-496B-BA93-20BA3FCF1FB1}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="D30" firstHeaderRow="0" firstDataRow="0" firstDataCol="0" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="16">
+    <pivotField axis="axisPage" showAll="0">
+      <items count="17">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="9"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="10"/>
+        <item x="8"/>
+        <item x="14"/>
+        <item x="12"/>
+        <item x="3"/>
+        <item x="15"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="9" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <pageFields count="1">
+    <pageField fld="0" hier="-1"/>
+  </pageFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{53B5388F-02D5-4DD9-8188-58334394F7C1}" name="PivotTable9" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="K3:L7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="9" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Average" fld="11" baseField="0" baseItem="0" numFmtId="165"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="27">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{69D2ADC1-2991-4FC7-9CA9-CAF7A5967579}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="F16:G20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="9" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="10" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="5">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1C4E3AE5-F52A-418F-9C54-B54E76FDEF67}" name="PivotTable11" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="R2:S6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0">
+      <items count="15">
+        <item x="13"/>
+        <item x="12"/>
+        <item x="11"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="9" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Average" fld="11" subtotal="average" baseField="2" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="2" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{55CBBF39-7A0B-4B5F-B4B0-A658124677FA}" name="PivotTable10" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="N2:O10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0">
+      <items count="15">
+        <item x="13"/>
+        <item x="12"/>
+        <item x="11"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="9" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Average" fld="11" subtotal="average" baseField="1" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="2">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="4">
+    <chartFormat chart="2" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{165F3E78-6375-46CE-9624-48443D408C22}" name="PivotTable1" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="3">
+  <location ref="B2:C9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="17">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="9"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="10"/>
+        <item x="8"/>
+        <item x="14"/>
+        <item x="12"/>
+        <item x="3"/>
+        <item x="15"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
+    <pivotField compact="0" numFmtId="9" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+    <i i="6">
+      <x v="6"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="7">
+    <dataField name="Sum of Jul-21" fld="3" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Aug-21" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Sep-21" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Oct-21" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Nov-21" fld="7" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Dec-21" fld="8" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Jan-22" fld="9" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="3">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="9">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5383FE3D-DBE8-44CD-ADF5-9A09D777DD32}" name="PivotTable7" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+  <location ref="M16:M17" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField compact="0" showAll="0"/>
+    <pivotField compact="0" showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="9" showAll="0"/>
+    <pivotField compact="0" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of MoM" fld="14" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2D4E6CDA-203E-4D14-B3EC-C27B3E2A842C}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="F2:G10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -13060,10 +14310,10 @@
     <dataField name="Sum of Total" fld="10" baseField="0" baseItem="0" numFmtId="167"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="7">
+    <format dxfId="6">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="5">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6" selected="0">
@@ -13077,7 +14327,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="4">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -13185,8 +14435,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{26FF0945-102D-481A-92C5-E05B89D80EC3}" name="PivotTable8" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{26FF0945-102D-481A-92C5-E05B89D80EC3}" name="PivotTable8" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="M21:M22" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="16">
     <pivotField dataField="1" showAll="0"/>
@@ -13239,1196 +14489,6 @@
   <dataFields count="1">
     <dataField name="Count of MOVIE" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0D4AFFF-2BFF-415B-98D2-4EC608BED0AA}" name="PivotTable5" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
-  <location ref="J16:J17" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField compact="0" showAll="0"/>
-    <pivotField compact="0" showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="6"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField dataField="1" compact="0" numFmtId="164" showAll="0">
-      <items count="15">
-        <item x="13"/>
-        <item x="12"/>
-        <item x="11"/>
-        <item x="10"/>
-        <item x="9"/>
-        <item x="8"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="9" showAll="0"/>
-    <pivotField compact="0" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total" fld="10" baseField="0" baseItem="0" numFmtId="164"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="8">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F156695-00A6-4622-942C-8A4E46F4AA06}" name="PivotTable6" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="J21:J22" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="6"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="9" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Average" fld="11" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="9">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D4BBF573-D747-496B-BA93-20BA3FCF1FB1}" name="PivotTable4" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="D30" firstHeaderRow="0" firstDataRow="0" firstDataCol="0" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="16">
-    <pivotField axis="axisPage" showAll="0">
-      <items count="17">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item x="9"/>
-        <item x="4"/>
-        <item x="7"/>
-        <item x="5"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="10"/>
-        <item x="8"/>
-        <item x="14"/>
-        <item x="12"/>
-        <item x="3"/>
-        <item x="15"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="9" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <pageFields count="1">
-    <pageField fld="0" hier="-1"/>
-  </pageFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{53B5388F-02D5-4DD9-8188-58334394F7C1}" name="PivotTable9" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="K3:L7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="9" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Average" fld="11" baseField="0" baseItem="0" numFmtId="165"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="27">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1C4E3AE5-F52A-418F-9C54-B54E76FDEF67}" name="PivotTable11" cacheId="6" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="R2:S6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="6"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField dataField="1" numFmtId="164" showAll="0">
-      <items count="15">
-        <item x="13"/>
-        <item x="12"/>
-        <item x="11"/>
-        <item x="10"/>
-        <item x="9"/>
-        <item x="8"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="9" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Average" fld="11" subtotal="average" baseField="2" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="0">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="1">
-    <chartFormat chart="2" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{55CBBF39-7A0B-4B5F-B4B0-A658124677FA}" name="PivotTable10" cacheId="6" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="N2:O10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="6"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField dataField="1" numFmtId="164" showAll="0">
-      <items count="15">
-        <item x="13"/>
-        <item x="12"/>
-        <item x="11"/>
-        <item x="10"/>
-        <item x="9"/>
-        <item x="8"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="9" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="8">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Average" fld="11" subtotal="average" baseField="1" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="1">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="4">
-    <chartFormat chart="2" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="9">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="10">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5383FE3D-DBE8-44CD-ADF5-9A09D777DD32}" name="PivotTable7" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
-  <location ref="M16:M17" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField compact="0" showAll="0"/>
-    <pivotField compact="0" showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="6"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" showAll="0"/>
-    <pivotField dataField="1" compact="0" numFmtId="9" showAll="0"/>
-    <pivotField compact="0" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of MoM" fld="14" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4D9962DE-38CB-4034-A1F8-9ADCEFCAE6F3}" name="PivotTable9" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="J26" firstHeaderRow="0" firstDataRow="0" firstDataCol="0" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="16">
-    <pivotField axis="axisPage" showAll="0">
-      <items count="17">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item x="9"/>
-        <item x="4"/>
-        <item x="7"/>
-        <item x="5"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="10"/>
-        <item x="8"/>
-        <item x="14"/>
-        <item x="12"/>
-        <item x="3"/>
-        <item x="15"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="6"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="9" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <pageFields count="1">
-    <pageField fld="0" hier="-1"/>
-  </pageFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6B138F6B-7AFC-4CD2-A1A3-926BBE22CE78}" name="PivotTable4" cacheId="6" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="J2:K9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="6"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0">
-      <items count="15">
-        <item x="13"/>
-        <item x="12"/>
-        <item x="11"/>
-        <item x="10"/>
-        <item x="9"/>
-        <item x="8"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="9" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
-    <i i="5">
-      <x v="5"/>
-    </i>
-    <i i="6">
-      <x v="6"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="7">
-    <dataField name="Average of Jul-21" fld="3" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="Average of Aug-21" fld="4" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="Average of Sep-21" fld="5" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="Average of Oct-21" fld="6" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="Average of Nov-21" fld="7" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="Average of Dec-21" fld="8" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="Average of Jan-22" fld="9" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="2">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="1">
-    <chartFormat chart="2" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{69D2ADC1-2991-4FC7-9CA9-CAF7A5967579}" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="F16:G20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="6"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="9" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total" fld="10" baseField="0" baseItem="0" numFmtId="164"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="3">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="5">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="5" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="6">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="7">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{165F3E78-6375-46CE-9624-48443D408C22}" name="PivotTable1" cacheId="6" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="3">
-  <location ref="B2:C9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="17">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item x="9"/>
-        <item x="4"/>
-        <item x="7"/>
-        <item x="5"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="10"/>
-        <item x="8"/>
-        <item x="14"/>
-        <item x="12"/>
-        <item x="3"/>
-        <item x="15"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="6"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
-    <pivotField compact="0" numFmtId="9" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
-    <i i="5">
-      <x v="5"/>
-    </i>
-    <i i="6">
-      <x v="6"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="7">
-    <dataField name="Sum of Jul-21" fld="3" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Aug-21" fld="4" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Sep-21" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Oct-21" fld="6" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Nov-21" fld="7" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Dec-21" fld="8" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Jan-22" fld="9" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="4">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="9">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="5">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="6">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="7">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -14870,12 +14930,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="2:12">
       <c r="B3" s="10" t="s">
@@ -15346,7 +15406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4F75E6-FCA5-4FE8-B964-2CD11B93EC1B}">
   <dimension ref="A2:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -15363,24 +15423,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="18.75">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1">
       <c r="A3" s="5" t="s">
@@ -16262,8 +16322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419EAC9E-4B08-4FC7-8F69-05D076D6ABCB}">
   <dimension ref="B2:S24"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16330,7 +16390,7 @@
       <c r="F3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="66">
+      <c r="G3" s="14">
         <v>75416</v>
       </c>
       <c r="J3" s="9" t="s">
@@ -16554,7 +16614,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="6:13">
+    <row r="17" spans="6:17">
       <c r="F17" s="9" t="s">
         <v>5</v>
       </c>
@@ -16568,15 +16628,18 @@
         <v>-0.21301260508443476</v>
       </c>
     </row>
-    <row r="18" spans="6:13">
+    <row r="18" spans="6:17">
       <c r="F18" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="7">
         <v>5411117</v>
       </c>
+      <c r="Q18" t="s">
+        <v>78</v>
+      </c>
     </row>
-    <row r="19" spans="6:13">
+    <row r="19" spans="6:17">
       <c r="F19" s="9" t="s">
         <v>11</v>
       </c>
@@ -16584,7 +16647,7 @@
         <v>2240742</v>
       </c>
     </row>
-    <row r="20" spans="6:13">
+    <row r="20" spans="6:17">
       <c r="F20" s="9" t="s">
         <v>40</v>
       </c>
@@ -16592,7 +16655,7 @@
         <v>15306092</v>
       </c>
     </row>
-    <row r="21" spans="6:13">
+    <row r="21" spans="6:17">
       <c r="J21" t="s">
         <v>56</v>
       </c>
@@ -16600,7 +16663,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="6:13">
+    <row r="22" spans="6:17">
       <c r="J22" s="7">
         <v>136661.53571428568</v>
       </c>
@@ -16608,7 +16671,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="6:13">
+    <row r="24" spans="6:17">
       <c r="J24" s="8" t="s">
         <v>0</v>
       </c>
@@ -16636,69 +16699,69 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:21" ht="15" customHeight="1">
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-      <c r="U3" s="20"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
     </row>
     <row r="4" spans="3:21" ht="15" customHeight="1">
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="20"/>
-      <c r="U4" s="20"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
     </row>
     <row r="5" spans="3:21" ht="15" customHeight="1">
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="20"/>
-      <c r="U5" s="20"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
     </row>
     <row r="7" spans="3:21">
       <c r="G7" s="19" t="s">
@@ -16738,133 +16801,133 @@
     </row>
     <row r="9" spans="3:21" ht="15.75" thickBot="1"/>
     <row r="10" spans="3:21" ht="19.5" thickBot="1">
-      <c r="G10" s="57" t="s">
+      <c r="G10" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="58"/>
-      <c r="I10" s="59"/>
-      <c r="K10" s="60" t="s">
+      <c r="H10" s="61"/>
+      <c r="I10" s="62"/>
+      <c r="K10" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="L10" s="61"/>
-      <c r="M10" s="62"/>
-      <c r="O10" s="63" t="s">
+      <c r="L10" s="64"/>
+      <c r="M10" s="65"/>
+      <c r="O10" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="P10" s="64"/>
-      <c r="Q10" s="65"/>
-      <c r="S10" s="16" t="s">
+      <c r="P10" s="67"/>
+      <c r="Q10" s="68"/>
+      <c r="S10" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="T10" s="17"/>
-      <c r="U10" s="18"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="22"/>
     </row>
     <row r="11" spans="3:21">
-      <c r="G11" s="21">
+      <c r="G11" s="24">
         <f>GETPIVOTDATA("Total",BuildDB!$J$16)</f>
         <v>15306092</v>
       </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="23"/>
-      <c r="K11" s="30">
+      <c r="H11" s="25"/>
+      <c r="I11" s="26"/>
+      <c r="K11" s="33">
         <f>GETPIVOTDATA("Average",BuildDB!$J$21)</f>
         <v>136661.53571428568</v>
       </c>
-      <c r="L11" s="31"/>
-      <c r="M11" s="32"/>
-      <c r="O11" s="39">
+      <c r="L11" s="34"/>
+      <c r="M11" s="35"/>
+      <c r="O11" s="42">
         <f>GETPIVOTDATA("MoM",BuildDB!$M$16)</f>
         <v>-0.21301260508443476</v>
       </c>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="41"/>
-      <c r="S11" s="48">
+      <c r="P11" s="43"/>
+      <c r="Q11" s="44"/>
+      <c r="S11" s="51">
         <f>GETPIVOTDATA("MOVIE",BuildDB!$M$21)</f>
         <v>16</v>
       </c>
-      <c r="T11" s="49"/>
-      <c r="U11" s="50"/>
+      <c r="T11" s="52"/>
+      <c r="U11" s="53"/>
     </row>
     <row r="12" spans="3:21">
-      <c r="G12" s="24"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="26"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="35"/>
-      <c r="O12" s="42"/>
-      <c r="P12" s="43"/>
-      <c r="Q12" s="44"/>
-      <c r="S12" s="51"/>
-      <c r="T12" s="52"/>
-      <c r="U12" s="53"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="29"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="38"/>
+      <c r="O12" s="45"/>
+      <c r="P12" s="46"/>
+      <c r="Q12" s="47"/>
+      <c r="S12" s="54"/>
+      <c r="T12" s="55"/>
+      <c r="U12" s="56"/>
     </row>
     <row r="13" spans="3:21">
-      <c r="G13" s="24"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="26"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="35"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="43"/>
-      <c r="Q13" s="44"/>
-      <c r="S13" s="51"/>
-      <c r="T13" s="52"/>
-      <c r="U13" s="53"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="29"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="38"/>
+      <c r="O13" s="45"/>
+      <c r="P13" s="46"/>
+      <c r="Q13" s="47"/>
+      <c r="S13" s="54"/>
+      <c r="T13" s="55"/>
+      <c r="U13" s="56"/>
     </row>
     <row r="14" spans="3:21" ht="15.75" thickBot="1">
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="29"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="38"/>
-      <c r="O14" s="45"/>
-      <c r="P14" s="46"/>
-      <c r="Q14" s="47"/>
-      <c r="S14" s="54"/>
-      <c r="T14" s="55"/>
-      <c r="U14" s="56"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="32"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="41"/>
+      <c r="O14" s="48"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="50"/>
+      <c r="S14" s="57"/>
+      <c r="T14" s="58"/>
+      <c r="U14" s="59"/>
     </row>
     <row r="15" spans="3:21">
       <c r="G15" s="12"/>
     </row>
     <row r="26" spans="3:6">
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
     </row>
     <row r="27" spans="3:6">
-      <c r="C27" s="68" t="s">
+      <c r="C27" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
     </row>
     <row r="28" spans="3:6">
-      <c r="C28" s="67"/>
+      <c r="C28" s="15"/>
       <c r="D28" s="8" t="s">
         <v>0</v>
       </c>
       <c r="E28" t="s">
         <v>73</v>
       </c>
-      <c r="F28" s="67"/>
+      <c r="F28" s="15"/>
     </row>
     <row r="29" spans="3:6">
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="67"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
     </row>
     <row r="30" spans="3:6">
-      <c r="C30" s="67"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
     </row>
     <row r="47" spans="7:21">
       <c r="G47" s="19" t="s">
@@ -16940,11 +17003,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="G47:U48"/>
-    <mergeCell ref="G85:U86"/>
-    <mergeCell ref="S10:U10"/>
-    <mergeCell ref="G7:U8"/>
     <mergeCell ref="C3:U5"/>
     <mergeCell ref="G11:I14"/>
     <mergeCell ref="K11:M14"/>
@@ -16953,6 +17011,11 @@
     <mergeCell ref="G10:I10"/>
     <mergeCell ref="K10:M10"/>
     <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="G47:U48"/>
+    <mergeCell ref="G85:U86"/>
+    <mergeCell ref="S10:U10"/>
+    <mergeCell ref="G7:U8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId2"/>

</xml_diff>